<commit_message>
ADD: lock-free queue only for single producer called SingleProducerQueue and its test case and perf test
</commit_message>
<xml_diff>
--- a/report/LockFreeQueuePerfTestResult.xlsx
+++ b/report/LockFreeQueuePerfTestResult.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13">
   <si>
     <t>producer</t>
   </si>
@@ -38,7 +38,8 @@
     <t>BAD</t>
   </si>
   <si>
-    <t>push operation time = pop operation time = 100*1000;
+    <t>capacity of lock-free queue = 10*1000,
+push operation time = pop operation time = 100*1000;
 skip time = 5;
  repeat time = 100;</t>
   </si>
@@ -62,6 +63,11 @@
   <si>
     <t>with spin lock, the performance of blocking std queue win all cases 
 except when producer number is 1</t>
+  </si>
+  <si>
+    <t>push operation time = pop operation time = 100*1000;
+skip time = 5;
+ repeat time = 100;</t>
   </si>
   <si>
     <t xml:space="preserve">system info:
@@ -1090,7 +1096,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+      <selection activeCell="I2" sqref="I2:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2257,7 +2263,7 @@
         <v/>
       </c>
       <c r="I2" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -2541,7 +2547,7 @@
         <v/>
       </c>
       <c r="I11" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -3131,7 +3137,7 @@
         <v>Bad</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>

</xml_diff>

<commit_message>
ADD: user manual in README.md
</commit_message>
<xml_diff>
--- a/report/LockFreeQueuePerfTestResult.xlsx
+++ b/report/LockFreeQueuePerfTestResult.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14">
   <si>
     <t>producer</t>
   </si>
@@ -26,7 +26,7 @@
     <t>LockFreeQueue</t>
   </si>
   <si>
-    <t>BlockingStlQueue</t>
+    <t>BlockingStlQueueWithMutex</t>
   </si>
   <si>
     <t>Ratio</t>
@@ -63,6 +63,9 @@
   <si>
     <t>with spin lock, the performance of blocking std queue win all cases 
 except when producer number is 1</t>
+  </si>
+  <si>
+    <t>BlockingStlQueue</t>
   </si>
   <si>
     <t>push operation time = pop operation time = 100*1000;
@@ -1096,12 +1099,13 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:N7"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="3" max="3" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="12.625"/>
     <col min="6" max="6" width="9" style="3"/>
   </cols>
@@ -2225,7 +2229,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -2263,7 +2267,7 @@
         <v/>
       </c>
       <c r="I2" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -2547,7 +2551,7 @@
         <v/>
       </c>
       <c r="I11" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -3137,7 +3141,7 @@
         <v>Bad</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>

</xml_diff>